<commit_message>
Inhalte der letzten Einheit + Client File
</commit_message>
<xml_diff>
--- a/Dokumente/Lerngruppe_Uebersicht.xlsx
+++ b/Dokumente/Lerngruppe_Uebersicht.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="150" windowWidth="20115" windowHeight="8190"/>
+    <workbookView xWindow="600" yWindow="150" windowWidth="20115" windowHeight="8190" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="56">
   <si>
     <t>KW</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>ListContainer, Zusammenfassung</t>
-  </si>
-  <si>
     <t>KatalogNr</t>
   </si>
   <si>
@@ -174,7 +171,19 @@
     <t>Bemerkung</t>
   </si>
   <si>
-    <t>Mangelndes Interesse, Störung der Lerneinheit(Lärm, Abspielen von Videos,….)--&gt; Dinic, Bogdanovic,Coric,Kulancic,….</t>
+    <t>Entfallen/Weihnachtsfeier</t>
+  </si>
+  <si>
+    <t>Ferien</t>
+  </si>
+  <si>
+    <t>Mangelndes Interesse, Störung der Lerneinheit(Lärm, Abspielen von Videos,….)--&gt; Dinic, Bogdanovic,Kulancic,….</t>
+  </si>
+  <si>
+    <t>HTMLFrame, TagContainer</t>
+  </si>
+  <si>
+    <t>Abstrakte Klasse</t>
   </si>
 </sst>
 </file>
@@ -313,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -371,6 +380,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +729,7 @@
         <v>13</v>
       </c>
       <c r="I1" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -743,7 +755,7 @@
         <v>41613</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -761,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>12</v>
@@ -770,10 +782,10 @@
         <v>41620</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -792,7 +804,9 @@
       <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="9" t="s">
+        <v>51</v>
+      </c>
       <c r="G4" s="6">
         <v>41627</v>
       </c>
@@ -812,10 +826,10 @@
       <c r="D5" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="9"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="G5" s="6">
         <v>41634</v>
       </c>
@@ -835,10 +849,10 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="9"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="9" t="s">
+        <v>52</v>
+      </c>
       <c r="G6" s="6">
         <v>41641</v>
       </c>
@@ -859,7 +873,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="6">
@@ -882,7 +896,7 @@
         <v>7</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="6">
@@ -905,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13">
@@ -928,7 +942,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="22">
@@ -978,13 +992,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -992,10 +1006,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,10 +1017,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1014,10 +1028,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1025,10 +1039,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1036,10 +1050,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1047,10 +1061,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1058,10 +1072,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1069,10 +1083,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1080,10 +1094,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1091,10 +1105,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1102,10 +1116,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1113,10 +1127,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1124,10 +1138,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1135,10 +1149,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1146,10 +1160,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1157,10 +1171,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1168,10 +1182,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1179,10 +1193,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1190,10 +1204,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1201,10 +1215,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1212,10 +1226,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,10 +1237,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1234,10 +1248,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1245,10 +1259,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1260,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C251"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="I50" sqref="I50"/>
+    <sheetView tabSelected="1" topLeftCell="A132" workbookViewId="0">
+      <selection activeCell="C146" sqref="C146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,10 +1290,10 @@
         <v>2</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1295,13 +1309,13 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1309,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="23"/>
     </row>
@@ -1318,7 +1332,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" s="24"/>
     </row>
@@ -1327,7 +1341,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" s="24"/>
     </row>
@@ -1336,10 +1350,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1347,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C8" s="24"/>
     </row>
@@ -1356,10 +1370,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1367,7 +1381,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="24"/>
     </row>
@@ -1376,7 +1390,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="24"/>
     </row>
@@ -1385,7 +1399,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="25"/>
     </row>
@@ -1394,7 +1408,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="24"/>
     </row>
@@ -1403,7 +1417,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="24"/>
     </row>
@@ -1412,7 +1426,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="24"/>
     </row>
@@ -1421,7 +1435,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="24"/>
     </row>
@@ -1430,7 +1444,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="25"/>
     </row>
@@ -1439,7 +1453,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="24"/>
     </row>
@@ -1448,10 +1462,10 @@
         <v>16</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1459,7 +1473,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="24"/>
     </row>
@@ -1468,7 +1482,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="24"/>
     </row>
@@ -1477,10 +1491,10 @@
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1488,7 +1502,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="24"/>
     </row>
@@ -1497,7 +1511,7 @@
         <v>21</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C24" s="24"/>
     </row>
@@ -1506,7 +1520,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="24"/>
     </row>
@@ -1515,7 +1529,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="24"/>
     </row>
@@ -1524,7 +1538,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="26"/>
     </row>
@@ -1538,10 +1552,10 @@
         <v>2</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1552,18 +1566,18 @@
         <v>41620</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C31" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1571,7 +1585,7 @@
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C32" s="23"/>
     </row>
@@ -1580,7 +1594,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C33" s="24"/>
     </row>
@@ -1589,7 +1603,7 @@
         <v>3</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" s="24"/>
     </row>
@@ -1598,7 +1612,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C35" s="24"/>
     </row>
@@ -1607,7 +1621,7 @@
         <v>5</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" s="24"/>
     </row>
@@ -1616,10 +1630,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C37" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,7 +1641,7 @@
         <v>7</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C38" s="24"/>
     </row>
@@ -1636,7 +1650,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C39" s="24"/>
     </row>
@@ -1645,7 +1659,7 @@
         <v>9</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C40" s="25"/>
     </row>
@@ -1654,7 +1668,7 @@
         <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C41" s="24"/>
     </row>
@@ -1663,7 +1677,7 @@
         <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C42" s="24"/>
     </row>
@@ -1672,7 +1686,7 @@
         <v>12</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C43" s="24"/>
     </row>
@@ -1681,7 +1695,7 @@
         <v>13</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C44" s="24"/>
     </row>
@@ -1690,7 +1704,7 @@
         <v>14</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C45" s="25"/>
     </row>
@@ -1699,7 +1713,7 @@
         <v>15</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C46" s="24"/>
     </row>
@@ -1708,10 +1722,10 @@
         <v>16</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C47" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1719,10 +1733,10 @@
         <v>17</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C48" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1730,7 +1744,7 @@
         <v>18</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C49" s="24"/>
     </row>
@@ -1739,10 +1753,10 @@
         <v>19</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C50" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1750,7 +1764,7 @@
         <v>20</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C51" s="24"/>
     </row>
@@ -1759,7 +1773,7 @@
         <v>21</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C52" s="24"/>
     </row>
@@ -1768,7 +1782,7 @@
         <v>22</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="24"/>
     </row>
@@ -1777,7 +1791,7 @@
         <v>23</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="24"/>
     </row>
@@ -1786,7 +1800,7 @@
         <v>24</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55" s="24"/>
     </row>
@@ -1796,10 +1810,10 @@
         <v>2</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C57" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1815,13 +1829,13 @@
     </row>
     <row r="59" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B59" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C59" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -1829,7 +1843,7 @@
         <v>1</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C60" s="5"/>
     </row>
@@ -1838,7 +1852,7 @@
         <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C61" s="2"/>
     </row>
@@ -1847,7 +1861,7 @@
         <v>3</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C62" s="2"/>
     </row>
@@ -1856,7 +1870,7 @@
         <v>4</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C63" s="2"/>
     </row>
@@ -1865,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C64" s="2"/>
     </row>
@@ -1874,7 +1888,7 @@
         <v>6</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C65" s="2"/>
     </row>
@@ -1883,7 +1897,7 @@
         <v>7</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C66" s="2"/>
     </row>
@@ -1892,7 +1906,7 @@
         <v>8</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C67" s="2"/>
     </row>
@@ -1901,7 +1915,7 @@
         <v>9</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C68" s="16"/>
     </row>
@@ -1910,7 +1924,7 @@
         <v>10</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C69" s="2"/>
     </row>
@@ -1919,7 +1933,7 @@
         <v>11</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C70" s="2"/>
     </row>
@@ -1928,7 +1942,7 @@
         <v>12</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C71" s="2"/>
     </row>
@@ -1937,7 +1951,7 @@
         <v>13</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C72" s="2"/>
     </row>
@@ -1946,7 +1960,7 @@
         <v>14</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C73" s="16"/>
     </row>
@@ -1955,7 +1969,7 @@
         <v>15</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C74" s="2"/>
     </row>
@@ -1964,7 +1978,7 @@
         <v>16</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C75" s="2"/>
     </row>
@@ -1973,7 +1987,7 @@
         <v>17</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C76" s="2"/>
     </row>
@@ -1982,7 +1996,7 @@
         <v>18</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C77" s="2"/>
     </row>
@@ -1991,7 +2005,7 @@
         <v>19</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C78" s="2"/>
     </row>
@@ -2000,7 +2014,7 @@
         <v>20</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C79" s="2"/>
     </row>
@@ -2009,7 +2023,7 @@
         <v>21</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C80" s="2"/>
     </row>
@@ -2018,7 +2032,7 @@
         <v>22</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C81" s="2"/>
     </row>
@@ -2027,7 +2041,7 @@
         <v>23</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C82" s="2"/>
     </row>
@@ -2036,7 +2050,7 @@
         <v>24</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C83" s="2"/>
     </row>
@@ -2046,10 +2060,10 @@
         <v>2</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2060,18 +2074,18 @@
         <v>41634</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B87" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C87" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2079,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C88" s="5"/>
     </row>
@@ -2088,7 +2102,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C89" s="2"/>
     </row>
@@ -2097,7 +2111,7 @@
         <v>3</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C90" s="2"/>
     </row>
@@ -2106,7 +2120,7 @@
         <v>4</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C91" s="2"/>
     </row>
@@ -2115,7 +2129,7 @@
         <v>5</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C92" s="2"/>
     </row>
@@ -2124,7 +2138,7 @@
         <v>6</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C93" s="2"/>
     </row>
@@ -2133,7 +2147,7 @@
         <v>7</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C94" s="2"/>
     </row>
@@ -2142,7 +2156,7 @@
         <v>8</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C95" s="2"/>
     </row>
@@ -2151,7 +2165,7 @@
         <v>9</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C96" s="16"/>
     </row>
@@ -2160,7 +2174,7 @@
         <v>10</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C97" s="2"/>
     </row>
@@ -2169,7 +2183,7 @@
         <v>11</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C98" s="2"/>
     </row>
@@ -2178,7 +2192,7 @@
         <v>12</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C99" s="2"/>
     </row>
@@ -2187,7 +2201,7 @@
         <v>13</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C100" s="2"/>
     </row>
@@ -2196,7 +2210,7 @@
         <v>14</v>
       </c>
       <c r="B101" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C101" s="16"/>
     </row>
@@ -2205,7 +2219,7 @@
         <v>15</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C102" s="2"/>
     </row>
@@ -2214,7 +2228,7 @@
         <v>16</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C103" s="2"/>
     </row>
@@ -2223,7 +2237,7 @@
         <v>17</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C104" s="2"/>
     </row>
@@ -2232,7 +2246,7 @@
         <v>18</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C105" s="2"/>
     </row>
@@ -2241,7 +2255,7 @@
         <v>19</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C106" s="2"/>
     </row>
@@ -2250,7 +2264,7 @@
         <v>20</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C107" s="2"/>
     </row>
@@ -2259,7 +2273,7 @@
         <v>21</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C108" s="2"/>
     </row>
@@ -2268,7 +2282,7 @@
         <v>22</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C109" s="2"/>
     </row>
@@ -2277,7 +2291,7 @@
         <v>23</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C110" s="2"/>
     </row>
@@ -2286,7 +2300,7 @@
         <v>24</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C111" s="2"/>
     </row>
@@ -2296,10 +2310,10 @@
         <v>2</v>
       </c>
       <c r="B113" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C113" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2310,18 +2324,18 @@
         <v>41641</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A115" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B115" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C115" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C115" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -2329,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C116" s="5"/>
     </row>
@@ -2338,7 +2352,7 @@
         <v>2</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C117" s="2"/>
     </row>
@@ -2347,7 +2361,7 @@
         <v>3</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C118" s="2"/>
     </row>
@@ -2356,7 +2370,7 @@
         <v>4</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C119" s="2"/>
     </row>
@@ -2365,7 +2379,7 @@
         <v>5</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C120" s="2"/>
     </row>
@@ -2374,7 +2388,7 @@
         <v>6</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C121" s="2"/>
     </row>
@@ -2383,7 +2397,7 @@
         <v>7</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C122" s="2"/>
     </row>
@@ -2392,7 +2406,7 @@
         <v>8</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C123" s="2"/>
     </row>
@@ -2401,7 +2415,7 @@
         <v>9</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C124" s="16"/>
     </row>
@@ -2410,7 +2424,7 @@
         <v>10</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C125" s="2"/>
     </row>
@@ -2419,7 +2433,7 @@
         <v>11</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C126" s="2"/>
     </row>
@@ -2428,7 +2442,7 @@
         <v>12</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C127" s="2"/>
     </row>
@@ -2437,7 +2451,7 @@
         <v>13</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C128" s="2"/>
     </row>
@@ -2446,7 +2460,7 @@
         <v>14</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C129" s="16"/>
     </row>
@@ -2455,7 +2469,7 @@
         <v>15</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C130" s="2"/>
     </row>
@@ -2464,7 +2478,7 @@
         <v>16</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C131" s="2"/>
     </row>
@@ -2473,7 +2487,7 @@
         <v>17</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C132" s="2"/>
     </row>
@@ -2482,7 +2496,7 @@
         <v>18</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C133" s="2"/>
     </row>
@@ -2491,7 +2505,7 @@
         <v>19</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C134" s="2"/>
     </row>
@@ -2500,7 +2514,7 @@
         <v>20</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C135" s="2"/>
     </row>
@@ -2509,7 +2523,7 @@
         <v>21</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C136" s="2"/>
     </row>
@@ -2518,7 +2532,7 @@
         <v>22</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C137" s="2"/>
     </row>
@@ -2527,7 +2541,7 @@
         <v>23</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C138" s="2"/>
     </row>
@@ -2536,7 +2550,7 @@
         <v>24</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C139" s="2"/>
     </row>
@@ -2546,10 +2560,10 @@
         <v>2</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C141" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2560,18 +2574,18 @@
         <v>41648</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
     </row>
     <row r="143" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B143" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C143" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C143" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
@@ -2579,227 +2593,243 @@
         <v>1</v>
       </c>
       <c r="B144" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C144" s="5"/>
+        <v>16</v>
+      </c>
+      <c r="C144" s="23"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
         <v>2</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C145" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="C145" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
         <v>3</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C146" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="C146" s="24"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
         <v>4</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C147" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="C147" s="24"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
         <v>5</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C148" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="C148" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
         <v>6</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C149" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="C149" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
         <v>7</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C150" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="C150" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
         <v>8</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C151" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="C151" s="24"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" s="16">
         <v>9</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C152" s="16"/>
+        <v>24</v>
+      </c>
+      <c r="C152" s="25"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
         <v>10</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C153" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="C153" s="24"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
         <v>11</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C154" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C154" s="24"/>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
         <v>12</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C155" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="C155" s="24"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
         <v>13</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C156" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="C156" s="24"/>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" s="16">
         <v>14</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C157" s="16"/>
+        <v>29</v>
+      </c>
+      <c r="C157" s="25"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>15</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C158" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="C158" s="24"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>16</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C159" s="2"/>
+        <v>31</v>
+      </c>
+      <c r="C159" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>17</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C160" s="2"/>
+        <v>32</v>
+      </c>
+      <c r="C160" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>18</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C161" s="2"/>
+        <v>33</v>
+      </c>
+      <c r="C161" s="24"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
         <v>19</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C162" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="C162" s="24"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
         <v>20</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C163" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C163" s="24" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
         <v>21</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C164" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C164" s="24"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
         <v>22</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C165" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C165" s="24"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
         <v>23</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C166" s="2"/>
+        <v>38</v>
+      </c>
+      <c r="C166" s="24"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
         <v>24</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C167" s="2"/>
-    </row>
-    <row r="168" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+        <v>39</v>
+      </c>
+      <c r="C167" s="24"/>
+    </row>
+    <row r="168" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C168" s="28"/>
+    </row>
     <row r="169" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A169" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B169" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C169" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2810,18 +2840,18 @@
         <v>41655</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A171" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B171" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C171" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C171" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
@@ -2829,7 +2859,7 @@
         <v>1</v>
       </c>
       <c r="B172" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C172" s="5"/>
     </row>
@@ -2838,7 +2868,7 @@
         <v>2</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C173" s="2"/>
     </row>
@@ -2847,7 +2877,7 @@
         <v>3</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C174" s="2"/>
     </row>
@@ -2856,7 +2886,7 @@
         <v>4</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C175" s="2"/>
     </row>
@@ -2865,7 +2895,7 @@
         <v>5</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C176" s="2"/>
     </row>
@@ -2874,7 +2904,7 @@
         <v>6</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C177" s="2"/>
     </row>
@@ -2883,7 +2913,7 @@
         <v>7</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C178" s="2"/>
     </row>
@@ -2892,7 +2922,7 @@
         <v>8</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C179" s="2"/>
     </row>
@@ -2901,7 +2931,7 @@
         <v>9</v>
       </c>
       <c r="B180" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C180" s="16"/>
     </row>
@@ -2910,7 +2940,7 @@
         <v>10</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C181" s="2"/>
     </row>
@@ -2919,7 +2949,7 @@
         <v>11</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C182" s="2"/>
     </row>
@@ -2928,7 +2958,7 @@
         <v>12</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C183" s="2"/>
     </row>
@@ -2937,7 +2967,7 @@
         <v>13</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C184" s="2"/>
     </row>
@@ -2946,7 +2976,7 @@
         <v>14</v>
       </c>
       <c r="B185" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C185" s="16"/>
     </row>
@@ -2955,7 +2985,7 @@
         <v>15</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C186" s="2"/>
     </row>
@@ -2964,7 +2994,7 @@
         <v>16</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C187" s="2"/>
     </row>
@@ -2973,7 +3003,7 @@
         <v>17</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C188" s="2"/>
     </row>
@@ -2982,7 +3012,7 @@
         <v>18</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C189" s="2"/>
     </row>
@@ -2991,7 +3021,7 @@
         <v>19</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C190" s="2"/>
     </row>
@@ -3000,7 +3030,7 @@
         <v>20</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C191" s="2"/>
     </row>
@@ -3009,7 +3039,7 @@
         <v>21</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C192" s="2"/>
     </row>
@@ -3018,7 +3048,7 @@
         <v>22</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C193" s="2"/>
     </row>
@@ -3027,7 +3057,7 @@
         <v>23</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C194" s="2"/>
     </row>
@@ -3036,7 +3066,7 @@
         <v>24</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C195" s="2"/>
     </row>
@@ -3046,10 +3076,10 @@
         <v>2</v>
       </c>
       <c r="B197" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C197" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3060,18 +3090,18 @@
         <v>41662</v>
       </c>
       <c r="C198" s="11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B199" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C199" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C199" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
@@ -3079,7 +3109,7 @@
         <v>1</v>
       </c>
       <c r="B200" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C200" s="5"/>
     </row>
@@ -3088,7 +3118,7 @@
         <v>2</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C201" s="2"/>
     </row>
@@ -3097,7 +3127,7 @@
         <v>3</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C202" s="2"/>
     </row>
@@ -3106,7 +3136,7 @@
         <v>4</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C203" s="2"/>
     </row>
@@ -3115,7 +3145,7 @@
         <v>5</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C204" s="2"/>
     </row>
@@ -3124,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C205" s="2"/>
     </row>
@@ -3133,7 +3163,7 @@
         <v>7</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C206" s="2"/>
     </row>
@@ -3142,7 +3172,7 @@
         <v>8</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C207" s="2"/>
     </row>
@@ -3151,7 +3181,7 @@
         <v>9</v>
       </c>
       <c r="B208" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C208" s="16"/>
     </row>
@@ -3160,7 +3190,7 @@
         <v>10</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C209" s="2"/>
     </row>
@@ -3169,7 +3199,7 @@
         <v>11</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C210" s="2"/>
     </row>
@@ -3178,7 +3208,7 @@
         <v>12</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C211" s="2"/>
     </row>
@@ -3187,7 +3217,7 @@
         <v>13</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C212" s="2"/>
     </row>
@@ -3196,7 +3226,7 @@
         <v>14</v>
       </c>
       <c r="B213" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C213" s="16"/>
     </row>
@@ -3205,7 +3235,7 @@
         <v>15</v>
       </c>
       <c r="B214" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C214" s="2"/>
     </row>
@@ -3214,7 +3244,7 @@
         <v>16</v>
       </c>
       <c r="B215" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C215" s="2"/>
     </row>
@@ -3223,7 +3253,7 @@
         <v>17</v>
       </c>
       <c r="B216" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C216" s="2"/>
     </row>
@@ -3232,7 +3262,7 @@
         <v>18</v>
       </c>
       <c r="B217" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C217" s="2"/>
     </row>
@@ -3241,7 +3271,7 @@
         <v>19</v>
       </c>
       <c r="B218" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C218" s="2"/>
     </row>
@@ -3250,7 +3280,7 @@
         <v>20</v>
       </c>
       <c r="B219" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C219" s="2"/>
     </row>
@@ -3259,7 +3289,7 @@
         <v>21</v>
       </c>
       <c r="B220" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C220" s="2"/>
     </row>
@@ -3268,7 +3298,7 @@
         <v>22</v>
       </c>
       <c r="B221" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C221" s="2"/>
     </row>
@@ -3277,7 +3307,7 @@
         <v>23</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C222" s="2"/>
     </row>
@@ -3286,7 +3316,7 @@
         <v>24</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C223" s="2"/>
     </row>
@@ -3296,10 +3326,10 @@
         <v>2</v>
       </c>
       <c r="B225" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C225" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="226" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3310,18 +3340,18 @@
         <v>41669</v>
       </c>
       <c r="C226" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="227" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A227" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B227" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C227" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C227" s="17" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
@@ -3329,7 +3359,7 @@
         <v>1</v>
       </c>
       <c r="B228" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C228" s="5"/>
     </row>
@@ -3338,7 +3368,7 @@
         <v>2</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C229" s="2"/>
     </row>
@@ -3347,7 +3377,7 @@
         <v>3</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C230" s="2"/>
     </row>
@@ -3356,7 +3386,7 @@
         <v>4</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C231" s="2"/>
     </row>
@@ -3365,7 +3395,7 @@
         <v>5</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C232" s="2"/>
     </row>
@@ -3374,7 +3404,7 @@
         <v>6</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C233" s="2"/>
     </row>
@@ -3383,7 +3413,7 @@
         <v>7</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C234" s="2"/>
     </row>
@@ -3392,7 +3422,7 @@
         <v>8</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C235" s="2"/>
     </row>
@@ -3401,7 +3431,7 @@
         <v>9</v>
       </c>
       <c r="B236" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C236" s="16"/>
     </row>
@@ -3410,7 +3440,7 @@
         <v>10</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C237" s="2"/>
     </row>
@@ -3419,7 +3449,7 @@
         <v>11</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C238" s="2"/>
     </row>
@@ -3428,7 +3458,7 @@
         <v>12</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C239" s="2"/>
     </row>
@@ -3437,7 +3467,7 @@
         <v>13</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C240" s="2"/>
     </row>
@@ -3446,7 +3476,7 @@
         <v>14</v>
       </c>
       <c r="B241" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C241" s="16"/>
     </row>
@@ -3455,7 +3485,7 @@
         <v>15</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C242" s="2"/>
     </row>
@@ -3464,7 +3494,7 @@
         <v>16</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C243" s="2"/>
     </row>
@@ -3473,7 +3503,7 @@
         <v>17</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C244" s="2"/>
     </row>
@@ -3482,7 +3512,7 @@
         <v>18</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C245" s="2"/>
     </row>
@@ -3491,7 +3521,7 @@
         <v>19</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C246" s="2"/>
     </row>
@@ -3500,7 +3530,7 @@
         <v>20</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C247" s="2"/>
     </row>
@@ -3509,7 +3539,7 @@
         <v>21</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C248" s="2"/>
     </row>
@@ -3518,7 +3548,7 @@
         <v>22</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C249" s="2"/>
     </row>
@@ -3527,7 +3557,7 @@
         <v>23</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C250" s="2"/>
     </row>
@@ -3536,7 +3566,7 @@
         <v>24</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C251" s="2"/>
     </row>

</xml_diff>